<commit_message>
Updated script to accomodate for multiple series
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://opinium-my.sharepoint.com/personal/meeaadbharooch_opinium_com/Documents/Documents/Meeaad/Python Scripts/Charting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECC563B1-7A55-4008-AC67-8D767E10E4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{ECC563B1-7A55-4008-AC67-8D767E10E4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FE6BAB5-1A81-4E4B-8418-1C47EE41775F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-16320" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6072" yWindow="-108" windowWidth="17280" windowHeight="8964" firstSheet="17" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRONT PAGE" sheetId="20" r:id="rId1"/>
@@ -3612,6 +3612,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -6759,6 +6760,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -9906,6 +9908,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -13053,6 +13056,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -16200,6 +16204,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -19347,6 +19352,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -22492,13 +22498,14 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A3"/>
+      <selection pane="bottomRight" sqref="A1:AQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -25637,13 +25644,14 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:AQ19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A3"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -27738,13 +27746,14 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:AQ29"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A3"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -31144,6 +31153,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:AQ25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -34305,13 +34315,14 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:AQ31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A3"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -37974,9 +37985,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -40597,6 +40609,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AQ19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -42698,13 +42711,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AQ21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A3"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -45060,6 +45074,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AQ19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -47161,13 +47176,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -47862,6 +47878,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -51009,6 +51026,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AQ27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>